<commit_message>
readme moved and bug report
</commit_message>
<xml_diff>
--- a/musicVis-master/Bug Reports/Bug Reports.xlsx
+++ b/musicVis-master/Bug Reports/Bug Reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\Motlias\Univestiy\Intro to Programming\Music vis bug reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamb\Desktop\GitHub Repositories\Music-Vis\musicVis-master\Bug Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E7012F-3D4F-4628-AEE4-391BB24A1F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9EB8F2-F9BC-4EDB-9AC0-7AD85DFC307E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA863988-A299-45A2-94A5-8EFFB4D4E4C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BA863988-A299-45A2-94A5-8EFFB4D4E4C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Bug Reports</t>
   </si>
@@ -114,6 +112,21 @@
   </si>
   <si>
     <t>v0.4</t>
+  </si>
+  <si>
+    <t>buzzwire volume glitch</t>
+  </si>
+  <si>
+    <t>when the mouse is too far from the line the volume is set to 0, and when move to another visualser it stays at 0</t>
+  </si>
+  <si>
+    <t>command added to the select vis key press, sound.setVolume(vol);</t>
+  </si>
+  <si>
+    <t>V0.5</t>
+  </si>
+  <si>
+    <t>bug found by Deniz</t>
   </si>
 </sst>
 </file>
@@ -834,27 +847,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B237802-B303-4DC5-9228-BEF9CCF86BE5}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="91.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="91.7265625" customWidth="1"/>
+    <col min="4" max="4" width="50.54296875" customWidth="1"/>
+    <col min="6" max="6" width="31.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -877,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
@@ -896,7 +909,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
@@ -915,7 +928,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="2:8" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="134.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
@@ -934,7 +947,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="2:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
@@ -953,7 +966,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="2:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
@@ -972,16 +985,28 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+    <row r="9" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="12"/>
@@ -990,7 +1015,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="12"/>
@@ -999,7 +1024,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="12"/>
@@ -1008,7 +1033,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
@@ -1017,7 +1042,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
@@ -1026,7 +1051,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="2"/>
       <c r="D15" s="12"/>
@@ -1035,7 +1060,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="11"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
@@ -1044,7 +1069,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="11"/>
       <c r="C17" s="2"/>
       <c r="D17" s="12"/>
@@ -1053,7 +1078,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="2"/>
       <c r="D18" s="5"/>
@@ -1062,7 +1087,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D19" s="8"/>
     </row>
   </sheetData>

</xml_diff>